<commit_message>
onto week10 pb 4
</commit_message>
<xml_diff>
--- a/week10/ClassAssignments.xlsx
+++ b/week10/ClassAssignments.xlsx
@@ -1,14 +1,72 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21721"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23416"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1280" yWindow="1840" windowWidth="19340" windowHeight="15280" tabRatio="500"/>
+    <workbookView xWindow="23800" yWindow="0" windowWidth="22220" windowHeight="26260" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="solver_adj" localSheetId="0" hidden="1">Sheet1!$B$50:$C$89</definedName>
+    <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
+    <definedName name="solver_drv" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_eng" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_lhs1" localSheetId="0" hidden="1">Sheet1!$B$100</definedName>
+    <definedName name="solver_lhs10" localSheetId="0" hidden="1">Sheet1!$D$50:$D$89</definedName>
+    <definedName name="solver_lhs2" localSheetId="0" hidden="1">Sheet1!$B$50:$C$89</definedName>
+    <definedName name="solver_lhs3" localSheetId="0" hidden="1">Sheet1!$B$59</definedName>
+    <definedName name="solver_lhs4" localSheetId="0" hidden="1">Sheet1!$B$69</definedName>
+    <definedName name="solver_lhs5" localSheetId="0" hidden="1">Sheet1!$B$91:$C$91</definedName>
+    <definedName name="solver_lhs6" localSheetId="0" hidden="1">Sheet1!$B$92:$C$92</definedName>
+    <definedName name="solver_lhs7" localSheetId="0" hidden="1">Sheet1!$C$100</definedName>
+    <definedName name="solver_lhs8" localSheetId="0" hidden="1">Sheet1!$C$50</definedName>
+    <definedName name="solver_lhs9" localSheetId="0" hidden="1">Sheet1!$C$89</definedName>
+    <definedName name="solver_lin" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_mip" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_mni" localSheetId="0" hidden="1">30</definedName>
+    <definedName name="solver_mrt" localSheetId="0" hidden="1">0.075</definedName>
+    <definedName name="solver_msl" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_num" localSheetId="0" hidden="1">10</definedName>
+    <definedName name="solver_opt" localSheetId="0" hidden="1">Sheet1!$B$95</definedName>
+    <definedName name="solver_pre" localSheetId="0" hidden="1">0.000000001</definedName>
+    <definedName name="solver_rbv" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel1" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_rel10" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_rel2" localSheetId="0" hidden="1">4</definedName>
+    <definedName name="solver_rel3" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_rel4" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_rel5" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_rel6" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel7" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_rel8" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_rel9" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_rhs1" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_rhs10" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rhs2" localSheetId="0" hidden="1">integer</definedName>
+    <definedName name="solver_rhs3" localSheetId="0" hidden="1">Sheet1!$C$60</definedName>
+    <definedName name="solver_rhs4" localSheetId="0" hidden="1">Sheet1!$B$70</definedName>
+    <definedName name="solver_rhs5" localSheetId="0" hidden="1">20</definedName>
+    <definedName name="solver_rhs6" localSheetId="0" hidden="1">12</definedName>
+    <definedName name="solver_rhs7" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_rhs8" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rhs9" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_rsd" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_scl" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_ssz" localSheetId="0" hidden="1">100</definedName>
+    <definedName name="solver_tim" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_tol" localSheetId="0" hidden="1">0.01</definedName>
+    <definedName name="solver_typ" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_ver" localSheetId="0" hidden="1">2</definedName>
+  </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -19,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="18">
   <si>
     <t>CLASS ASSIGNMENTS IN AN ELEMENTARY SCHOOL</t>
   </si>
@@ -44,12 +102,42 @@
   <si>
     <t>F</t>
   </si>
+  <si>
+    <t>Class 1</t>
+  </si>
+  <si>
+    <t>Class 2</t>
+  </si>
+  <si>
+    <t>Student</t>
+  </si>
+  <si>
+    <t>Objective</t>
+  </si>
+  <si>
+    <t>got pref?</t>
+  </si>
+  <si>
+    <t>Students 10 and 11 must be separate</t>
+  </si>
+  <si>
+    <t>2 students from 4, 9, 15, 25, 30, and 36 in same class</t>
+  </si>
+  <si>
+    <t>Students 20 and 21 in same class</t>
+  </si>
+  <si>
+    <t>Student 1 in class 2</t>
+  </si>
+  <si>
+    <t>Student 40 in class 2</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -70,13 +158,41 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="9">
@@ -174,10 +290,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -212,8 +332,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -543,10 +675,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D44"/>
+  <dimension ref="A1:E103"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="A102" sqref="A102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -554,32 +686,35 @@
     <col min="1" max="1" width="17.6640625" customWidth="1"/>
     <col min="2" max="2" width="30.83203125" customWidth="1"/>
     <col min="3" max="3" width="30" customWidth="1"/>
-    <col min="4" max="4" width="34.1640625" customWidth="1"/>
+    <col min="4" max="5" width="34.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18">
+    <row r="1" spans="1:5" ht="18">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
-    </row>
-    <row r="2" spans="1:4" ht="18">
+      <c r="E1" s="1"/>
+    </row>
+    <row r="2" spans="1:5" ht="18">
       <c r="A2" s="2"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
-    </row>
-    <row r="3" spans="1:4" ht="19" thickBot="1">
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:5" ht="19" thickBot="1">
       <c r="A3" s="11" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="1:4" ht="19" thickBot="1">
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:5" ht="19" thickBot="1">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -592,8 +727,9 @@
       <c r="D4" s="5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="18">
+      <c r="E4" s="14"/>
+    </row>
+    <row r="5" spans="1:5" ht="18">
       <c r="A5" s="6">
         <v>1</v>
       </c>
@@ -606,8 +742,12 @@
       <c r="D5" s="7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="18">
+      <c r="E5" s="15">
+        <f>IF(D5="M",1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="18">
       <c r="A6" s="6">
         <v>2</v>
       </c>
@@ -620,8 +760,12 @@
       <c r="D6" s="7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="18">
+      <c r="E6" s="15">
+        <f t="shared" ref="E6:E44" si="0">IF(D6="M",1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="18">
       <c r="A7" s="6">
         <v>3</v>
       </c>
@@ -634,8 +778,12 @@
       <c r="D7" s="7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="18">
+      <c r="E7" s="15">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="18">
       <c r="A8" s="6">
         <v>4</v>
       </c>
@@ -648,8 +796,12 @@
       <c r="D8" s="7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="18">
+      <c r="E8" s="15">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="18">
       <c r="A9" s="6">
         <v>5</v>
       </c>
@@ -662,8 +814,12 @@
       <c r="D9" s="7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="18">
+      <c r="E9" s="15">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="18">
       <c r="A10" s="6">
         <v>6</v>
       </c>
@@ -676,8 +832,12 @@
       <c r="D10" s="7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="18">
+      <c r="E10" s="15">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="18">
       <c r="A11" s="6">
         <v>7</v>
       </c>
@@ -690,8 +850,12 @@
       <c r="D11" s="7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="18">
+      <c r="E11" s="15">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="18">
       <c r="A12" s="6">
         <v>8</v>
       </c>
@@ -704,8 +868,12 @@
       <c r="D12" s="7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="18">
+      <c r="E12" s="15">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="18">
       <c r="A13" s="6">
         <v>9</v>
       </c>
@@ -718,8 +886,12 @@
       <c r="D13" s="7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="18">
+      <c r="E13" s="15">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="18">
       <c r="A14" s="6">
         <v>10</v>
       </c>
@@ -732,8 +904,12 @@
       <c r="D14" s="7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" ht="18">
+      <c r="E14" s="15">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="18">
       <c r="A15" s="6">
         <v>11</v>
       </c>
@@ -746,8 +922,12 @@
       <c r="D15" s="7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" ht="18">
+      <c r="E15" s="15">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="18">
       <c r="A16" s="6">
         <v>12</v>
       </c>
@@ -760,8 +940,12 @@
       <c r="D16" s="7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="18">
+      <c r="E16" s="15">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="18">
       <c r="A17" s="6">
         <v>13</v>
       </c>
@@ -774,8 +958,12 @@
       <c r="D17" s="7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" ht="18">
+      <c r="E17" s="15">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="18">
       <c r="A18" s="6">
         <v>14</v>
       </c>
@@ -788,8 +976,12 @@
       <c r="D18" s="7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" ht="18">
+      <c r="E18" s="15">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="18">
       <c r="A19" s="6">
         <v>15</v>
       </c>
@@ -802,8 +994,12 @@
       <c r="D19" s="7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" ht="18">
+      <c r="E19" s="15">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="18">
       <c r="A20" s="6">
         <v>16</v>
       </c>
@@ -816,8 +1012,12 @@
       <c r="D20" s="7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" ht="18">
+      <c r="E20" s="15">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="18">
       <c r="A21" s="6">
         <v>17</v>
       </c>
@@ -830,8 +1030,12 @@
       <c r="D21" s="7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" ht="18">
+      <c r="E21" s="15">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="18">
       <c r="A22" s="6">
         <v>18</v>
       </c>
@@ -844,8 +1048,12 @@
       <c r="D22" s="7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" ht="18">
+      <c r="E22" s="15">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="18">
       <c r="A23" s="6">
         <v>19</v>
       </c>
@@ -858,8 +1066,12 @@
       <c r="D23" s="7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" ht="18">
+      <c r="E23" s="15">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="18">
       <c r="A24" s="6">
         <v>20</v>
       </c>
@@ -872,8 +1084,12 @@
       <c r="D24" s="7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" ht="18">
+      <c r="E24" s="15">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="18">
       <c r="A25" s="6">
         <v>21</v>
       </c>
@@ -886,8 +1102,12 @@
       <c r="D25" s="7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" ht="18">
+      <c r="E25" s="15">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="18">
       <c r="A26" s="6">
         <v>22</v>
       </c>
@@ -900,8 +1120,12 @@
       <c r="D26" s="7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" ht="18">
+      <c r="E26" s="15">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="18">
       <c r="A27" s="6">
         <v>23</v>
       </c>
@@ -914,8 +1138,12 @@
       <c r="D27" s="7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" ht="18">
+      <c r="E27" s="15">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="18">
       <c r="A28" s="6">
         <v>24</v>
       </c>
@@ -928,8 +1156,12 @@
       <c r="D28" s="7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" ht="18">
+      <c r="E28" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="18">
       <c r="A29" s="6">
         <v>25</v>
       </c>
@@ -942,8 +1174,12 @@
       <c r="D29" s="7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" ht="18">
+      <c r="E29" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="18">
       <c r="A30" s="6">
         <v>26</v>
       </c>
@@ -956,8 +1192,12 @@
       <c r="D30" s="7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" ht="18">
+      <c r="E30" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="18">
       <c r="A31" s="6">
         <v>27</v>
       </c>
@@ -970,8 +1210,12 @@
       <c r="D31" s="7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" ht="18">
+      <c r="E31" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="18">
       <c r="A32" s="6">
         <v>28</v>
       </c>
@@ -984,8 +1228,12 @@
       <c r="D32" s="7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" ht="18">
+      <c r="E32" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="18">
       <c r="A33" s="6">
         <v>29</v>
       </c>
@@ -998,8 +1246,12 @@
       <c r="D33" s="7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" ht="18">
+      <c r="E33" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="18">
       <c r="A34" s="6">
         <v>30</v>
       </c>
@@ -1012,8 +1264,12 @@
       <c r="D34" s="7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" ht="18">
+      <c r="E34" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="18">
       <c r="A35" s="6">
         <v>31</v>
       </c>
@@ -1026,8 +1282,12 @@
       <c r="D35" s="7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" ht="18">
+      <c r="E35" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="18">
       <c r="A36" s="6">
         <v>32</v>
       </c>
@@ -1040,8 +1300,12 @@
       <c r="D36" s="7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" ht="18">
+      <c r="E36" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="18">
       <c r="A37" s="6">
         <v>33</v>
       </c>
@@ -1054,8 +1318,12 @@
       <c r="D37" s="7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" ht="18">
+      <c r="E37" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="18">
       <c r="A38" s="6">
         <v>34</v>
       </c>
@@ -1068,8 +1336,12 @@
       <c r="D38" s="7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" ht="18">
+      <c r="E38" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="18">
       <c r="A39" s="6">
         <v>35</v>
       </c>
@@ -1082,8 +1354,12 @@
       <c r="D39" s="7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" ht="18">
+      <c r="E39" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="18">
       <c r="A40" s="6">
         <v>36</v>
       </c>
@@ -1096,8 +1372,12 @@
       <c r="D40" s="7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" ht="18">
+      <c r="E40" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="18">
       <c r="A41" s="6">
         <v>37</v>
       </c>
@@ -1110,8 +1390,12 @@
       <c r="D41" s="7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" ht="18">
+      <c r="E41" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="18">
       <c r="A42" s="6">
         <v>38</v>
       </c>
@@ -1124,8 +1408,12 @@
       <c r="D42" s="7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" ht="18">
+      <c r="E42" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="18">
       <c r="A43" s="6">
         <v>39</v>
       </c>
@@ -1138,8 +1426,12 @@
       <c r="D43" s="7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" ht="19" thickBot="1">
+      <c r="E43" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="19" thickBot="1">
       <c r="A44" s="8">
         <v>40</v>
       </c>
@@ -1152,9 +1444,859 @@
       <c r="D44" s="10" t="s">
         <v>7</v>
       </c>
+      <c r="E44" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" t="s">
+        <v>10</v>
+      </c>
+      <c r="B49" t="s">
+        <v>8</v>
+      </c>
+      <c r="C49" t="s">
+        <v>9</v>
+      </c>
+      <c r="E49" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50">
+        <v>1</v>
+      </c>
+      <c r="B50" s="13">
+        <v>0</v>
+      </c>
+      <c r="C50" s="13">
+        <v>1</v>
+      </c>
+      <c r="D50">
+        <f>SUM(B50:C50)</f>
+        <v>1</v>
+      </c>
+      <c r="E50">
+        <f>SUMPRODUCT(B50:C50,B5:C5)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51">
+        <v>2</v>
+      </c>
+      <c r="B51" s="13">
+        <v>0</v>
+      </c>
+      <c r="C51" s="13">
+        <v>1</v>
+      </c>
+      <c r="D51">
+        <f t="shared" ref="D51:D89" si="1">SUM(B51:C51)</f>
+        <v>1</v>
+      </c>
+      <c r="E51">
+        <f t="shared" ref="E51:E89" si="2">SUMPRODUCT(B51:C51,B6:C6)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52">
+        <v>3</v>
+      </c>
+      <c r="B52" s="13">
+        <v>0</v>
+      </c>
+      <c r="C52" s="13">
+        <v>1</v>
+      </c>
+      <c r="D52">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E52">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53">
+        <v>4</v>
+      </c>
+      <c r="B53" s="13">
+        <v>1</v>
+      </c>
+      <c r="C53" s="13">
+        <v>0</v>
+      </c>
+      <c r="D53">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E53">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54">
+        <v>5</v>
+      </c>
+      <c r="B54" s="13">
+        <v>1</v>
+      </c>
+      <c r="C54" s="13">
+        <v>0</v>
+      </c>
+      <c r="D54">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E54">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55">
+        <v>6</v>
+      </c>
+      <c r="B55" s="13">
+        <v>0</v>
+      </c>
+      <c r="C55" s="13">
+        <v>1</v>
+      </c>
+      <c r="D55">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E55">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56">
+        <v>7</v>
+      </c>
+      <c r="B56" s="13">
+        <v>1</v>
+      </c>
+      <c r="C56" s="13">
+        <v>0</v>
+      </c>
+      <c r="D56">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E56">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57">
+        <v>8</v>
+      </c>
+      <c r="B57" s="13">
+        <v>0</v>
+      </c>
+      <c r="C57" s="13">
+        <v>1</v>
+      </c>
+      <c r="D57">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E57">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58">
+        <v>9</v>
+      </c>
+      <c r="B58" s="13">
+        <v>1</v>
+      </c>
+      <c r="C58" s="13">
+        <v>0</v>
+      </c>
+      <c r="D58">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E58">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59">
+        <v>10</v>
+      </c>
+      <c r="B59" s="13">
+        <v>1</v>
+      </c>
+      <c r="C59" s="13">
+        <v>0</v>
+      </c>
+      <c r="D59">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E59">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60">
+        <v>11</v>
+      </c>
+      <c r="B60" s="13">
+        <v>0</v>
+      </c>
+      <c r="C60" s="13">
+        <v>1</v>
+      </c>
+      <c r="D60">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E60">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61">
+        <v>12</v>
+      </c>
+      <c r="B61" s="13">
+        <v>0</v>
+      </c>
+      <c r="C61" s="13">
+        <v>1</v>
+      </c>
+      <c r="D61">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E61">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62">
+        <v>13</v>
+      </c>
+      <c r="B62" s="13">
+        <v>1</v>
+      </c>
+      <c r="C62" s="13">
+        <v>0</v>
+      </c>
+      <c r="D62">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E62">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63">
+        <v>14</v>
+      </c>
+      <c r="B63" s="13">
+        <v>1</v>
+      </c>
+      <c r="C63" s="13">
+        <v>0</v>
+      </c>
+      <c r="D63">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E63">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64">
+        <v>15</v>
+      </c>
+      <c r="B64" s="13">
+        <v>1</v>
+      </c>
+      <c r="C64" s="13">
+        <v>0</v>
+      </c>
+      <c r="D64">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E64">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
+      <c r="A65">
+        <v>16</v>
+      </c>
+      <c r="B65" s="13">
+        <v>0</v>
+      </c>
+      <c r="C65" s="13">
+        <v>1</v>
+      </c>
+      <c r="D65">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E65">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
+      <c r="A66">
+        <v>17</v>
+      </c>
+      <c r="B66" s="13">
+        <v>1</v>
+      </c>
+      <c r="C66" s="13">
+        <v>0</v>
+      </c>
+      <c r="D66">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E66">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
+      <c r="A67">
+        <v>18</v>
+      </c>
+      <c r="B67" s="13">
+        <v>1</v>
+      </c>
+      <c r="C67" s="13">
+        <v>0</v>
+      </c>
+      <c r="D67">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E67">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5">
+      <c r="A68">
+        <v>19</v>
+      </c>
+      <c r="B68" s="13">
+        <v>1</v>
+      </c>
+      <c r="C68" s="13">
+        <v>0</v>
+      </c>
+      <c r="D68">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E68">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5">
+      <c r="A69">
+        <v>20</v>
+      </c>
+      <c r="B69" s="13">
+        <v>0</v>
+      </c>
+      <c r="C69" s="13">
+        <v>1</v>
+      </c>
+      <c r="D69">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E69">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5">
+      <c r="A70">
+        <v>21</v>
+      </c>
+      <c r="B70" s="13">
+        <v>0</v>
+      </c>
+      <c r="C70" s="13">
+        <v>1</v>
+      </c>
+      <c r="D70">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E70">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5">
+      <c r="A71">
+        <v>22</v>
+      </c>
+      <c r="B71" s="13">
+        <v>1</v>
+      </c>
+      <c r="C71" s="13">
+        <v>0</v>
+      </c>
+      <c r="D71">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E71">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5">
+      <c r="A72">
+        <v>23</v>
+      </c>
+      <c r="B72" s="13">
+        <v>0</v>
+      </c>
+      <c r="C72" s="13">
+        <v>1</v>
+      </c>
+      <c r="D72">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E72">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5">
+      <c r="A73">
+        <v>24</v>
+      </c>
+      <c r="B73" s="13">
+        <v>1</v>
+      </c>
+      <c r="C73" s="13">
+        <v>0</v>
+      </c>
+      <c r="D73">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E73">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5">
+      <c r="A74">
+        <v>25</v>
+      </c>
+      <c r="B74" s="13">
+        <v>0</v>
+      </c>
+      <c r="C74" s="13">
+        <v>1</v>
+      </c>
+      <c r="D74">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E74">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5">
+      <c r="A75">
+        <v>26</v>
+      </c>
+      <c r="B75" s="13">
+        <v>0</v>
+      </c>
+      <c r="C75" s="13">
+        <v>1</v>
+      </c>
+      <c r="D75">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E75">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5">
+      <c r="A76">
+        <v>27</v>
+      </c>
+      <c r="B76" s="13">
+        <v>0</v>
+      </c>
+      <c r="C76" s="13">
+        <v>1</v>
+      </c>
+      <c r="D76">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E76">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5">
+      <c r="A77">
+        <v>28</v>
+      </c>
+      <c r="B77" s="13">
+        <v>1</v>
+      </c>
+      <c r="C77" s="13">
+        <v>0</v>
+      </c>
+      <c r="D77">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E77">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5">
+      <c r="A78">
+        <v>29</v>
+      </c>
+      <c r="B78" s="13">
+        <v>0</v>
+      </c>
+      <c r="C78" s="13">
+        <v>1</v>
+      </c>
+      <c r="D78">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E78">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5">
+      <c r="A79">
+        <v>30</v>
+      </c>
+      <c r="B79" s="13">
+        <v>1</v>
+      </c>
+      <c r="C79" s="13">
+        <v>0</v>
+      </c>
+      <c r="D79">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E79">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5">
+      <c r="A80">
+        <v>31</v>
+      </c>
+      <c r="B80" s="13">
+        <v>0</v>
+      </c>
+      <c r="C80" s="13">
+        <v>1</v>
+      </c>
+      <c r="D80">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E80">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5">
+      <c r="A81">
+        <v>32</v>
+      </c>
+      <c r="B81" s="13">
+        <v>1</v>
+      </c>
+      <c r="C81" s="13">
+        <v>0</v>
+      </c>
+      <c r="D81">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E81">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5">
+      <c r="A82">
+        <v>33</v>
+      </c>
+      <c r="B82" s="13">
+        <v>1</v>
+      </c>
+      <c r="C82" s="13">
+        <v>0</v>
+      </c>
+      <c r="D82">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E82">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5">
+      <c r="A83">
+        <v>34</v>
+      </c>
+      <c r="B83" s="13">
+        <v>1</v>
+      </c>
+      <c r="C83" s="13">
+        <v>0</v>
+      </c>
+      <c r="D83">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E83">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5">
+      <c r="A84">
+        <v>35</v>
+      </c>
+      <c r="B84" s="13">
+        <v>0</v>
+      </c>
+      <c r="C84" s="13">
+        <v>1</v>
+      </c>
+      <c r="D84">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E84">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5">
+      <c r="A85">
+        <v>36</v>
+      </c>
+      <c r="B85" s="13">
+        <v>0</v>
+      </c>
+      <c r="C85" s="13">
+        <v>1</v>
+      </c>
+      <c r="D85">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E85">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5">
+      <c r="A86">
+        <v>37</v>
+      </c>
+      <c r="B86" s="13">
+        <v>1</v>
+      </c>
+      <c r="C86" s="13">
+        <v>0</v>
+      </c>
+      <c r="D86">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E86">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5">
+      <c r="A87">
+        <v>38</v>
+      </c>
+      <c r="B87" s="13">
+        <v>0</v>
+      </c>
+      <c r="C87" s="13">
+        <v>1</v>
+      </c>
+      <c r="D87">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E87">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5">
+      <c r="A88">
+        <v>39</v>
+      </c>
+      <c r="B88" s="13">
+        <v>1</v>
+      </c>
+      <c r="C88" s="13">
+        <v>0</v>
+      </c>
+      <c r="D88">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E88">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5">
+      <c r="A89">
+        <v>40</v>
+      </c>
+      <c r="B89" s="13">
+        <v>0</v>
+      </c>
+      <c r="C89" s="13">
+        <v>1</v>
+      </c>
+      <c r="D89">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E89">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5">
+      <c r="B91">
+        <f>SUM(B50:B89)</f>
+        <v>20</v>
+      </c>
+      <c r="C91">
+        <f>SUM(C50:C89)</f>
+        <v>20</v>
+      </c>
+      <c r="E91">
+        <f>SUMIF(E50:E89,"=2")</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5">
+      <c r="B92">
+        <f>SUMPRODUCT(B50:B89,$E$5:$E$44)</f>
+        <v>12</v>
+      </c>
+      <c r="C92">
+        <f>SUMPRODUCT(C50:C89,$E$5:$E$44)</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5">
+      <c r="A95" t="s">
+        <v>11</v>
+      </c>
+      <c r="B95" s="12">
+        <f>SUMPRODUCT(B50:C89,B5:C44)</f>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3">
+      <c r="A98" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3">
+      <c r="A99" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3">
+      <c r="B100">
+        <f>B53+B58+B64+B74+B79+B85</f>
+        <v>4</v>
+      </c>
+      <c r="C100">
+        <f>C53+C58+C64+C74+C79+C85</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3">
+      <c r="A101" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3">
+      <c r="A102" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3">
+      <c r="A103" t="s">
+        <v>17</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <ignoredErrors>
+    <ignoredError sqref="D50" formulaRange="1"/>
+  </ignoredErrors>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>